<commit_message>
add process cadastro produto
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13095"/>
+    <workbookView windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <t>AUTOMOTIVO</t>
   </si>
   <si>
-    <t>Caixa</t>
+    <t xml:space="preserve">Caixa  </t>
   </si>
   <si>
     <t>Não</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">BATERIAS  </t>
   </si>
   <si>
-    <t>KIT</t>
+    <t xml:space="preserve">KIT  </t>
   </si>
   <si>
     <t>ROTEADOR DE CGN THUNDER 4440 DC A10</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">CABOS  </t>
   </si>
   <si>
-    <t>Metro</t>
+    <t xml:space="preserve">Metro  </t>
   </si>
   <si>
     <t>Sim</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">CALÇADOS  </t>
   </si>
   <si>
-    <t>PACOTE</t>
+    <t xml:space="preserve">PACOTE  </t>
   </si>
   <si>
     <t>ROTEADOR DE CGN THUNDER 3350 DC A10</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">CAMBIUM  </t>
   </si>
   <si>
-    <t>PAR</t>
+    <t xml:space="preserve">PAR  </t>
   </si>
   <si>
     <t>ROTEADOR DE CGN THUNDER 1040 DC A10</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">COMPUTADORES E PERIFÉRICOS  </t>
   </si>
   <si>
-    <t>Unidade</t>
+    <t xml:space="preserve">Unidade  </t>
   </si>
   <si>
     <t>FONTE DE ALIMENTACAO DC 1000W P/ PTX-1001 JUNIPER</t>
@@ -9291,8 +9291,30 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9306,23 +9328,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9335,9 +9342,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9352,17 +9367,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9378,14 +9385,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9406,15 +9405,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9429,14 +9420,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -9451,7 +9451,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9463,13 +9487,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9481,97 +9619,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9583,55 +9631,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9660,17 +9660,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9678,8 +9672,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9695,15 +9689,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -9732,6 +9717,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -9745,49 +9745,46 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -9796,97 +9793,100 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -10278,7 +10278,7 @@
   <dimension ref="A1:H3043"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="7"/>

</xml_diff>